<commit_message>
functional, get links matched titles
</commit_message>
<xml_diff>
--- a/matches.xlsx
+++ b/matches.xlsx
@@ -1,42 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP EliteBook\OneDrive\A_Miscalaneus\Escritorio\Code\git_folder\images_downloader\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF2463D-8D4F-4DC2-BF7F-16B4503CAFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -59,17 +46,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -347,46 +330,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24.1796875" customWidth="1"/>
-    <col min="2" max="2" width="49.90625" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D9" s="1"/>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>